<commit_message>
scenarij za brisanje dojave
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/BrisanjeDojave.xlsx
+++ b/UseCaseIScenarij/BrisanjeDojave.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naida\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naida\Grupa5-MEN\UseCaseIScenarij\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -65,9 +65,6 @@
     <t>Navigacioni sistem</t>
   </si>
   <si>
-    <t>Kada je problem koji se nalazio na putevima rješen, korinik briše dojavu i mape se ažuriraju.</t>
-  </si>
-  <si>
     <t>Korisnik mora biti registrovan i prijavljen i mora biti onaj korisnik koji je objavio tu dojavu.</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Tok događaja:</t>
+  </si>
+  <si>
+    <t>Kada je problem koji se nalazio na putevima riješen, korisnik briše dojavu i mape se ažuriraju.</t>
   </si>
 </sst>
 </file>
@@ -158,20 +158,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,162 +454,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>